<commit_message>
Add release date, finalize production files for the release
</commit_message>
<xml_diff>
--- a/docs/ZSWatch.xlsx
+++ b/docs/ZSWatch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B27E531-FF2C-4AAF-AC1A-EF05EEF9D1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2D774-B77F-4292-BD67-67F7159200AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11595" yWindow="3075" windowWidth="22140" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10845" yWindow="0" windowWidth="22140" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="225">
   <si>
     <r>
       <t xml:space="preserve">Nummer
@@ -309,9 +309,6 @@
     <t>2.0.3</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>4u7</t>
   </si>
   <si>
@@ -330,18 +327,12 @@
     <t>C2</t>
   </si>
   <si>
-    <t>2u2</t>
-  </si>
-  <si>
     <t>0603YD225KAT2A</t>
   </si>
   <si>
     <t>581-0603YD225KAT2A</t>
   </si>
   <si>
-    <t>C3, C10, C18</t>
-  </si>
-  <si>
     <t>GRM188R61A106MAALD</t>
   </si>
   <si>
@@ -351,36 +342,24 @@
     <t>12</t>
   </si>
   <si>
-    <t>C4, C6, C7, C8, C9, C12, C14, C16, C17, C19, C20, C21</t>
-  </si>
-  <si>
     <t>06035C104KAT2A</t>
   </si>
   <si>
     <t>581-06035C104KAT2A</t>
   </si>
   <si>
-    <t>C5, C13</t>
-  </si>
-  <si>
     <t>GRM188C80J226ME15D</t>
   </si>
   <si>
     <t>81-GRM188C80J226ME15D</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>0603YC105JAT2A</t>
   </si>
   <si>
     <t>581-0603YC105JAT2A</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>220n</t>
   </si>
   <si>
@@ -471,9 +450,6 @@
     <t>BMI270</t>
   </si>
   <si>
-    <t>Package_LGA:LGA-14_3x2.5mm_P0.5mm_LayoutBorder3x4y</t>
-  </si>
-  <si>
     <t>Bosch</t>
   </si>
   <si>
@@ -579,9 +555,6 @@
     <t>LIS2MDLTR</t>
   </si>
   <si>
-    <t>Package_LGA:LGA-12_2x2mm_P0.5mm</t>
-  </si>
-  <si>
     <t>511-LIS2MDLTR</t>
   </si>
   <si>
@@ -744,9 +717,6 @@
     <t>603-RC0603FR-0710KL</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>S1, S2, S3, S4</t>
   </si>
   <si>
@@ -760,9 +730,6 @@
   </si>
   <si>
     <t>612-TL6340AF160Q</t>
-  </si>
-  <si>
-    <t>33</t>
   </si>
   <si>
     <t>BATTERY</t>
@@ -956,6 +923,48 @@
   </si>
   <si>
     <t>OK-24F024-04</t>
+  </si>
+  <si>
+    <t>C1, C5, C7, C8, C9, C10, C13, C15, C17, C19, C20, C21</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4, C11, C18</t>
+  </si>
+  <si>
+    <t>C6, C14</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>Package_LGA_Kampi:LGA-14_3x2.5mm_P0.5mm_LayoutBorder3x4y</t>
+  </si>
+  <si>
+    <t>Package_LGA_Kampi:LGA-12_2x2mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>AT25SL128A-MHE-T</t>
+  </si>
+  <si>
+    <t>DOCK</t>
+  </si>
+  <si>
+    <t>Pomagtor:RD90_LZH0230529-004_DJ-5PIN_PH2_54</t>
+  </si>
+  <si>
+    <t>RD90_LZH0230529-004_DJ-5PIN_PH2_54</t>
+  </si>
+  <si>
+    <t>Pomagtor</t>
   </si>
 </sst>
 </file>
@@ -1560,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1573,7 +1582,7 @@
     <col min="3" max="3" width="58.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="58.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="25" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
@@ -1596,11 +1605,11 @@
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="22" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -1609,7 +1618,7 @@
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="23">
@@ -1623,7 +1632,7 @@
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A4" s="35" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="17" t="s">
@@ -1636,11 +1645,11 @@
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A5" s="35" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="17" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="17"/>
@@ -1661,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>1</v>
@@ -1688,7 +1697,7 @@
         <v>9</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1696,25 +1705,25 @@
         <v>25</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="G8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>50</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>51</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>25</v>
@@ -1723,7 +1732,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1731,25 +1740,23 @@
         <v>26</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="G9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>55</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>25</v>
@@ -1758,7 +1765,7 @@
         <v>24</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1766,25 +1773,25 @@
         <v>27</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>56</v>
+        <v>213</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I10" s="20" t="s">
         <v>27</v>
@@ -1793,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="38.25">
@@ -1801,34 +1808,34 @@
         <v>29</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>60</v>
+        <v>211</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="F11" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1836,25 +1843,25 @@
         <v>31</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>26</v>
@@ -1863,7 +1870,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1871,25 +1878,25 @@
         <v>32</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="F13" s="20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>25</v>
@@ -1898,7 +1905,7 @@
         <v>24</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1906,25 +1913,25 @@
         <v>33</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>69</v>
+        <v>216</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>49</v>
-      </c>
       <c r="F14" s="20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>25</v>
@@ -1933,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1944,22 +1951,22 @@
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>25</v>
@@ -1968,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1979,22 +1986,22 @@
         <v>14</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>25</v>
@@ -2003,7 +2010,7 @@
         <v>24</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2014,22 +2021,22 @@
         <v>15</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>25</v>
@@ -2038,33 +2045,33 @@
         <v>24</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>25</v>
@@ -2073,33 +2080,33 @@
         <v>24</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>25</v>
@@ -2108,33 +2115,33 @@
         <v>24</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="20" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>93</v>
+        <v>220</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>25</v>
@@ -2143,33 +2150,33 @@
         <v>24</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="20" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>25</v>
@@ -2178,33 +2185,33 @@
         <v>24</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="20" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>25</v>
@@ -2213,33 +2220,33 @@
         <v>24</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="20" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>25</v>
@@ -2248,33 +2255,33 @@
         <v>24</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="20" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>25</v>
@@ -2283,33 +2290,33 @@
         <v>24</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="20" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>25</v>
@@ -2318,33 +2325,33 @@
         <v>24</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="20" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>25</v>
@@ -2353,15 +2360,15 @@
         <v>24</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>39</v>
@@ -2370,7 +2377,7 @@
         <v>40</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>39</v>
@@ -2388,33 +2395,33 @@
         <v>24</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="20" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>25</v>
@@ -2423,33 +2430,33 @@
         <v>24</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="20" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>25</v>
@@ -2458,33 +2465,33 @@
         <v>24</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="14" customFormat="1" ht="15">
       <c r="A30" s="20" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>26</v>
@@ -2493,33 +2500,33 @@
         <v>24</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="20" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>25</v>
@@ -2528,33 +2535,33 @@
         <v>24</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F32" s="20" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>26</v>
@@ -2563,33 +2570,33 @@
         <v>24</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="D33" s="20" t="s">
+      <c r="F33" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>163</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>172</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>25</v>
@@ -2598,33 +2605,33 @@
         <v>24</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="B34" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>176</v>
-      </c>
       <c r="G34" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>25</v>
@@ -2633,33 +2640,33 @@
         <v>24</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>173</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>182</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>31</v>
@@ -2668,33 +2675,33 @@
         <v>24</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>187</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>26</v>
@@ -2703,12 +2710,12 @@
         <v>24</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>43</v>
@@ -2717,19 +2724,19 @@
         <v>20</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="I37" s="20" t="s">
         <v>25</v>
@@ -2738,33 +2745,33 @@
         <v>24</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="20" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>29</v>
@@ -2773,203 +2780,248 @@
         <v>24</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="20" t="s">
-        <v>191</v>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A39" s="20">
+        <v>32</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>220</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>25</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
       <c r="J39" s="20" t="s">
         <v>24</v>
       </c>
       <c r="K39" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="20" t="s">
-        <v>197</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="20">
+        <v>33</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="E40" s="20"/>
+        <v>208</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>188</v>
+      </c>
       <c r="F40" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
+        <v>209</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>189</v>
+      </c>
       <c r="I40" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="J40" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="20">
+        <v>34</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>191</v>
+      </c>
       <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="F41" s="20" t="s">
+        <v>210</v>
+      </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+      <c r="I41" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="J41" s="20"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="28">
-        <v>34</v>
-      </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="D42" s="29" t="s">
+    <row r="42" spans="1:14">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="28">
+        <v>35</v>
+      </c>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="G42" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="I42" s="29" t="s">
+      <c r="E43" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="27">
-        <v>35</v>
-      </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="G43" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27">
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="27">
+        <v>36</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27">
         <v>1</v>
       </c>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="28">
-        <v>36</v>
-      </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-    </row>
-    <row r="48" spans="1:11" ht="15">
-      <c r="A48" s="24"/>
-      <c r="B48" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="28">
+        <v>37</v>
+      </c>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+    </row>
+    <row r="48" spans="1:14" ht="15">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
     </row>
     <row r="49" spans="1:4" ht="15">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
     </row>
     <row r="50" spans="1:4" ht="15">
-      <c r="A50" s="25"/>
-      <c r="B50" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
     </row>
     <row r="51" spans="1:4" ht="15">
-      <c r="A51" s="26"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="32" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C51" s="32"/>
       <c r="D51" s="32"/>
+    </row>
+    <row r="52" spans="1:4" ht="15">
+      <c r="A52" s="26"/>
+      <c r="B52" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" insertRows="0" deleteRows="0" sort="0"/>
   <mergeCells count="9">
-    <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B49:D49"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>

</xml_diff>

<commit_message>
- Streamline documentation and production files - Ready to merge
</commit_message>
<xml_diff>
--- a/docs/ZSWatch.xlsx
+++ b/docs/ZSWatch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2D774-B77F-4292-BD67-67F7159200AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E708B71-5B80-49F8-8FE2-60A98520970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10845" yWindow="0" windowWidth="22140" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22785" yWindow="4170" windowWidth="22140" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -1572,7 +1572,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1623,7 +1623,7 @@
       <c r="B3" s="34"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45194</v>
+        <v>45198</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>

</xml_diff>

<commit_message>
- Fix wrong part number for 10 uH inductors because the old part was a 1 uH inductor.
</commit_message>
<xml_diff>
--- a/docs/ZSWatch.xlsx
+++ b/docs/ZSWatch.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E708B71-5B80-49F8-8FE2-60A98520970A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D260076-BB6C-4FA7-9347-57AEB0134D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22785" yWindow="4170" windowWidth="22140" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -585,15 +585,6 @@
     <t>Inductor_SMD:L_0603_1608Metric</t>
   </si>
   <si>
-    <t>TAIYO YUDEN</t>
-  </si>
-  <si>
-    <t>LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
-    <t>963-LSCNB1608HKT1R0MD</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
@@ -965,6 +956,15 @@
   </si>
   <si>
     <t>Pomagtor</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>810-MLZ1608N100LT000</t>
   </si>
 </sst>
 </file>
@@ -1571,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1605,11 +1605,11 @@
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -1618,12 +1618,12 @@
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45198</v>
+        <v>45224</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A4" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="17" t="s">
@@ -1645,11 +1645,11 @@
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A5" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="17"/>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>1</v>
@@ -1697,7 +1697,7 @@
         <v>9</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1732,7 +1732,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1740,7 +1740,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20" t="s">
@@ -1765,7 +1765,7 @@
         <v>24</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1773,7 +1773,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>28</v>
@@ -1800,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="38.25">
@@ -1808,7 +1808,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>36</v>
@@ -1835,7 +1835,7 @@
         <v>24</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1843,7 +1843,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>42</v>
@@ -1870,7 +1870,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1878,7 +1878,7 @@
         <v>32</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>30</v>
@@ -1905,7 +1905,7 @@
         <v>24</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1913,7 +1913,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>63</v>
@@ -1940,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1975,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2010,7 +2010,7 @@
         <v>24</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2045,7 +2045,7 @@
         <v>24</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2080,7 +2080,7 @@
         <v>24</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -2115,7 +2115,7 @@
         <v>24</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -2135,7 +2135,7 @@
         <v>83</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>11</v>
@@ -2150,7 +2150,7 @@
         <v>24</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -2185,7 +2185,7 @@
         <v>24</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -2199,7 +2199,7 @@
         <v>92</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>93</v>
@@ -2220,7 +2220,7 @@
         <v>24</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2255,7 +2255,7 @@
         <v>24</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2290,7 +2290,7 @@
         <v>24</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2325,7 +2325,7 @@
         <v>24</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2360,7 +2360,7 @@
         <v>24</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2395,7 +2395,7 @@
         <v>24</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2409,7 +2409,7 @@
         <v>127</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>68</v>
@@ -2430,7 +2430,7 @@
         <v>24</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2465,7 +2465,7 @@
         <v>24</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="14" customFormat="1" ht="15">
@@ -2482,16 +2482,16 @@
         <v>137</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>26</v>
@@ -2500,33 +2500,33 @@
         <v>24</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="G31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="20" t="s">
         <v>143</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>146</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>25</v>
@@ -2535,33 +2535,33 @@
         <v>24</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>157</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>26</v>
@@ -2570,33 +2570,33 @@
         <v>24</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="20" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F33" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="G33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>163</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>25</v>
@@ -2605,33 +2605,33 @@
         <v>24</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="20" t="s">
         <v>165</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>168</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>25</v>
@@ -2640,33 +2640,33 @@
         <v>24</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>173</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>31</v>
@@ -2675,33 +2675,33 @@
         <v>24</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>178</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>26</v>
@@ -2710,12 +2710,12 @@
         <v>24</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>43</v>
@@ -2724,19 +2724,19 @@
         <v>20</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I37" s="20" t="s">
         <v>25</v>
@@ -2745,33 +2745,33 @@
         <v>24</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="C38" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E38" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="F38" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="20" t="s">
         <v>183</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>186</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>29</v>
@@ -2780,7 +2780,7 @@
         <v>24</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
@@ -2791,16 +2791,16 @@
         <v>22</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="D39" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>224</v>
-      </c>
       <c r="F39" s="20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2820,22 +2820,22 @@
         <v>23</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>25</v>
@@ -2844,7 +2844,7 @@
         <v>24</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2852,17 +2852,17 @@
         <v>34</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2891,22 +2891,22 @@
       </c>
       <c r="B43" s="29"/>
       <c r="C43" s="29" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D43" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G43" s="29" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I43" s="29" t="s">
         <v>25</v>
@@ -2920,15 +2920,15 @@
       </c>
       <c r="B44" s="27"/>
       <c r="C44" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H44" s="27"/>
       <c r="I44" s="27">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -2986,7 +2986,7 @@
     <row r="49" spans="1:4" ht="15">
       <c r="A49" s="24"/>
       <c r="B49" s="32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C49" s="32"/>
       <c r="D49" s="32"/>
@@ -2994,7 +2994,7 @@
     <row r="50" spans="1:4" ht="15">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
@@ -3002,7 +3002,7 @@
     <row r="51" spans="1:4" ht="15">
       <c r="A51" s="25"/>
       <c r="B51" s="32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C51" s="32"/>
       <c r="D51" s="32"/>
@@ -3010,7 +3010,7 @@
     <row r="52" spans="1:4" ht="15">
       <c r="A52" s="26"/>
       <c r="B52" s="32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C52" s="32"/>
       <c r="D52" s="32"/>

</xml_diff>

<commit_message>
- Update libraries to the latest version - Set correct version number in CHANGELOG - Cosmetic changes - Add new production files
Signed-off-by: Daniel Kampert <DanielKampert@kampis-elektroecke.de>
</commit_message>
<xml_diff>
--- a/docs/ZSWatch.xlsx
+++ b/docs/ZSWatch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D260076-BB6C-4FA7-9347-57AEB0134D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2D78F6-8B63-4BC2-A0B6-DFCD848C4E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -306,9 +306,6 @@
     <t>1M</t>
   </si>
   <si>
-    <t>2.0.3</t>
-  </si>
-  <si>
     <t>4u7</t>
   </si>
   <si>
@@ -965,6 +962,9 @@
   </si>
   <si>
     <t>810-MLZ1608N100LT000</t>
+  </si>
+  <si>
+    <t>2.0.4</t>
   </si>
 </sst>
 </file>
@@ -1571,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1605,11 +1605,11 @@
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A2" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -1618,12 +1618,12 @@
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A3" s="34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" s="34"/>
       <c r="C3" s="23">
         <f ca="1">TODAY()</f>
-        <v>45224</v>
+        <v>45228</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -1632,11 +1632,11 @@
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A4" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="17" t="s">
-        <v>45</v>
+        <v>224</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="17"/>
@@ -1645,11 +1645,11 @@
     </row>
     <row r="5" spans="1:11" s="10" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A5" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="17"/>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>1</v>
@@ -1697,7 +1697,7 @@
         <v>9</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1705,25 +1705,25 @@
         <v>25</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="E8" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="F8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="G8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>25</v>
@@ -1732,7 +1732,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1740,23 +1740,23 @@
         <v>26</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="F9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="20" t="s">
         <v>52</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>25</v>
@@ -1765,7 +1765,7 @@
         <v>24</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1773,25 +1773,25 @@
         <v>27</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="20" t="s">
         <v>54</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>55</v>
       </c>
       <c r="I10" s="20" t="s">
         <v>27</v>
@@ -1800,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="38.25">
@@ -1808,34 +1808,34 @@
         <v>29</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="F11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>58</v>
-      </c>
       <c r="I11" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1843,25 +1843,25 @@
         <v>31</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>21</v>
       </c>
       <c r="F12" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="20" t="s">
         <v>59</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>60</v>
       </c>
       <c r="I12" s="20" t="s">
         <v>26</v>
@@ -1870,7 +1870,7 @@
         <v>24</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1878,25 +1878,25 @@
         <v>32</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="F13" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>62</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>25</v>
@@ -1905,7 +1905,7 @@
         <v>24</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1913,25 +1913,25 @@
         <v>33</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="20" t="s">
+      <c r="G14" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>25</v>
@@ -1940,7 +1940,7 @@
         <v>24</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1951,22 +1951,22 @@
         <v>13</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="E15" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>134</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>25</v>
@@ -1975,7 +1975,7 @@
         <v>24</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1986,22 +1986,22 @@
         <v>14</v>
       </c>
       <c r="C16" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="E16" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="F16" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>25</v>
@@ -2010,7 +2010,7 @@
         <v>24</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2021,22 +2021,22 @@
         <v>15</v>
       </c>
       <c r="C17" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="E17" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="F17" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="20" t="s">
         <v>72</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>73</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>25</v>
@@ -2045,33 +2045,33 @@
         <v>24</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>75</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>25</v>
@@ -2080,33 +2080,33 @@
         <v>24</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>78</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>79</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>38</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>25</v>
@@ -2115,33 +2115,33 @@
         <v>24</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="F20" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>25</v>
@@ -2150,33 +2150,33 @@
         <v>24</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>91</v>
-      </c>
       <c r="C21" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="E21" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="F21" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>89</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>25</v>
@@ -2185,33 +2185,33 @@
         <v>24</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>96</v>
-      </c>
       <c r="C22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="F22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>94</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>25</v>
@@ -2220,33 +2220,33 @@
         <v>24</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>103</v>
-      </c>
       <c r="C23" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="E23" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="F23" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="G23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="20" t="s">
         <v>100</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>101</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>25</v>
@@ -2255,33 +2255,33 @@
         <v>24</v>
       </c>
       <c r="K23" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>109</v>
-      </c>
       <c r="C24" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="E24" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="F24" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>25</v>
@@ -2290,33 +2290,33 @@
         <v>24</v>
       </c>
       <c r="K24" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>113</v>
-      </c>
       <c r="C25" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>111</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>25</v>
@@ -2325,33 +2325,33 @@
         <v>24</v>
       </c>
       <c r="K25" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="C26" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="E26" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="20" t="s">
         <v>115</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>116</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>25</v>
@@ -2360,15 +2360,15 @@
         <v>24</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>124</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>39</v>
@@ -2377,7 +2377,7 @@
         <v>40</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>39</v>
@@ -2395,33 +2395,33 @@
         <v>24</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="C28" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="D28" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>128</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>25</v>
@@ -2430,33 +2430,33 @@
         <v>24</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="20" t="s">
-        <v>130</v>
-      </c>
       <c r="C29" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="E29" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="F29" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>122</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>25</v>
@@ -2465,33 +2465,33 @@
         <v>24</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="14" customFormat="1" ht="15">
       <c r="A30" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E30" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="20" t="s">
         <v>223</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>224</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>26</v>
@@ -2500,33 +2500,33 @@
         <v>24</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="F31" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="G31" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="20" t="s">
-        <v>143</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>25</v>
@@ -2535,33 +2535,33 @@
         <v>24</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="14" customFormat="1" ht="14.25" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>154</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>26</v>
@@ -2570,33 +2570,33 @@
         <v>24</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="D33" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="G33" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>160</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>25</v>
@@ -2605,33 +2605,33 @@
         <v>24</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="D34" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="D34" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" s="20" t="s">
-        <v>165</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>25</v>
@@ -2640,33 +2640,33 @@
         <v>24</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:14">
       <c r="A35" s="20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="D35" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" s="20" t="s">
         <v>169</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>170</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>31</v>
@@ -2675,33 +2675,33 @@
         <v>24</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="D36" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="20" t="s">
         <v>174</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>175</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>26</v>
@@ -2710,12 +2710,12 @@
         <v>24</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>43</v>
@@ -2724,19 +2724,19 @@
         <v>20</v>
       </c>
       <c r="D37" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E37" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="20" t="s">
-        <v>152</v>
-      </c>
       <c r="F37" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="20" t="s">
         <v>177</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>178</v>
       </c>
       <c r="I37" s="20" t="s">
         <v>25</v>
@@ -2745,33 +2745,33 @@
         <v>24</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
       <c r="A38" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B38" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="D38" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="F38" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>183</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>29</v>
@@ -2780,7 +2780,7 @@
         <v>24</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="13" customFormat="1" ht="14.25" customHeight="1">
@@ -2791,16 +2791,16 @@
         <v>22</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="E39" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="F39" s="20" t="s">
         <v>219</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>221</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>220</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
@@ -2820,22 +2820,22 @@
         <v>23</v>
       </c>
       <c r="C40" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="G40" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="20" t="s">
         <v>185</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="20" t="s">
-        <v>186</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>25</v>
@@ -2844,7 +2844,7 @@
         <v>24</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2852,17 +2852,17 @@
         <v>34</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C41" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>188</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -2891,22 +2891,22 @@
       </c>
       <c r="B43" s="29"/>
       <c r="C43" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="29" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F43" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="F43" s="29" t="s">
+      <c r="G43" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="29" t="s">
         <v>147</v>
-      </c>
-      <c r="G43" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="29" t="s">
-        <v>148</v>
       </c>
       <c r="I43" s="29" t="s">
         <v>25</v>
@@ -2920,15 +2920,15 @@
       </c>
       <c r="B44" s="27"/>
       <c r="C44" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="G44" s="27" t="s">
         <v>202</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>203</v>
       </c>
       <c r="H44" s="27"/>
       <c r="I44" s="27">
@@ -2943,7 +2943,7 @@
       </c>
       <c r="B45" s="29"/>
       <c r="C45" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -2986,7 +2986,7 @@
     <row r="49" spans="1:4" ht="15">
       <c r="A49" s="24"/>
       <c r="B49" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C49" s="32"/>
       <c r="D49" s="32"/>
@@ -2994,7 +2994,7 @@
     <row r="50" spans="1:4" ht="15">
       <c r="A50" s="30"/>
       <c r="B50" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
@@ -3002,7 +3002,7 @@
     <row r="51" spans="1:4" ht="15">
       <c r="A51" s="25"/>
       <c r="B51" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C51" s="32"/>
       <c r="D51" s="32"/>
@@ -3010,7 +3010,7 @@
     <row r="52" spans="1:4" ht="15">
       <c r="A52" s="26"/>
       <c r="B52" s="32" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C52" s="32"/>
       <c r="D52" s="32"/>

</xml_diff>